<commit_message>
Updated ZAF model - 2025-07-30 12:18
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9FA0F9-ED94-407D-879E-A6E141B58BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3877453-A4E4-4BE7-9B34-6C2821135AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -211,6 +211,24 @@
   </si>
   <si>
     <t>CCGT - CHP</t>
+  </si>
+  <si>
+    <t>~UC_T: FX</t>
+  </si>
+  <si>
+    <t>pset_pn</t>
+  </si>
+  <si>
+    <t>UCE_Solar capacity aggregation for peak</t>
+  </si>
+  <si>
+    <t>ElcAgg_Solar</t>
+  </si>
+  <si>
+    <t>UCE_Wind capacity aggregation for peak</t>
+  </si>
+  <si>
+    <t>ElcAgg_Wind</t>
   </si>
   <si>
     <t>EMBER Utilization Factors</t>
@@ -714,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AJ27"/>
+  <dimension ref="B1:AJ40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -762,19 +780,19 @@
     </row>
     <row r="2" spans="2:36" x14ac:dyDescent="0.45">
       <c r="F2" s="10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.45">
@@ -782,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4">
         <v>0.14488935721812435</v>
@@ -1275,6 +1293,72 @@
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L27" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1308,12 +1392,12 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" s="7">
         <v>2000</v>
@@ -1390,7 +1474,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>0.22831050228310504</v>
@@ -1990,12 +2074,12 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7">
         <v>2000</v>
@@ -2069,7 +2153,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B17" s="4">
         <v>0.22553478688815715</v>
@@ -2549,12 +2633,12 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B31" s="7">
         <v>2000</v>
@@ -2631,7 +2715,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B32" s="8">
         <v>210.67</v>
@@ -2708,7 +2792,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B33" s="9">
         <v>0.48</v>
@@ -3324,12 +3408,12 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B45" s="7">
         <v>2000</v>
@@ -3403,7 +3487,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B46" s="8">
         <v>190.01495599999998</v>
@@ -3477,7 +3561,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B47" s="9">
         <v>0.47752300000000003</v>
@@ -3957,12 +4041,12 @@
     </row>
     <row r="57" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A57" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A58" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B58" s="7">
         <v>2000</v>
@@ -4039,7 +4123,7 @@
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B59" s="9">
         <v>0.24</v>
@@ -4655,12 +4739,12 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A69" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B70" s="7">
         <v>2000</v>
@@ -4740,7 +4824,7 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B71" s="9">
         <v>0.2417</v>
@@ -5277,12 +5361,12 @@
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="85" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>27</v>
@@ -5362,10 +5446,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B87" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C87" s="9">
         <v>4</v>
@@ -5440,10 +5524,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B88" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C88" s="9">
         <v>4.7</v>

</xml_diff>